<commit_message>
the last of chapter 8!
</commit_message>
<xml_diff>
--- a/Spring_2017.xlsx
+++ b/Spring_2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Loans" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="134">
   <si>
     <t xml:space="preserve">Present Value = </t>
   </si>
@@ -434,13 +434,25 @@
     <t>deprication</t>
   </si>
   <si>
-    <t>training fee</t>
-  </si>
-  <si>
-    <t>savings</t>
-  </si>
-  <si>
     <t>machine life span</t>
+  </si>
+  <si>
+    <t>yearly savings</t>
+  </si>
+  <si>
+    <t>machine sale price</t>
+  </si>
+  <si>
+    <t>investment purchased</t>
+  </si>
+  <si>
+    <t>training costs</t>
+  </si>
+  <si>
+    <t>Inventory costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PV Sum = </t>
   </si>
 </sst>
 </file>
@@ -726,9 +738,6 @@
     <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -747,6 +756,9 @@
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1435,7 +1447,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,7 +1880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2255,8 +2267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2590,7 +2602,7 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>99</v>
@@ -2641,7 +2653,7 @@
         <v>95</v>
       </c>
       <c r="E16">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>100</v>
@@ -2698,54 +2710,54 @@
         <v>97</v>
       </c>
       <c r="E17" s="5">
-        <v>0.4</v>
+        <v>0.36</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>101</v>
       </c>
       <c r="H17">
         <f>$E$16*$E$17*H16</f>
-        <v>0.56799999999999995</v>
+        <v>0.53280000000000005</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:M17" si="2">$E$16*$E$17*I16</f>
-        <v>0.90879999999999994</v>
+        <f t="shared" ref="I17" si="2">$E$16*$E$17*I16</f>
+        <v>0.85248000000000002</v>
       </c>
       <c r="J17">
         <f t="shared" ref="J17" si="3">$E$16*$E$17*J16</f>
-        <v>0.54527999999999999</v>
+        <v>0.51148800000000005</v>
       </c>
       <c r="K17">
         <f t="shared" ref="K17" si="4">$E$16*$E$17*K16</f>
-        <v>0.32716799999999996</v>
+        <v>0.30689280000000002</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17" si="5">$E$16*$E$17*L16</f>
-        <v>0.32716799999999996</v>
+        <v>0.30689280000000002</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17" si="6">$E$16*$E$17*M16</f>
-        <v>0.16358400000000026</v>
+        <f>$E$16*$E$17*M16</f>
+        <v>0.15344640000000026</v>
       </c>
       <c r="N17">
-        <f t="shared" ref="N17" si="7">$E$16*$E$17*N16</f>
-        <v>0.56799999999999984</v>
+        <f t="shared" ref="N17" si="6">$E$16*$E$17*N16</f>
+        <v>0.53279999999999994</v>
       </c>
       <c r="O17">
-        <f t="shared" ref="O17" si="8">$E$16*$E$17*O16</f>
-        <v>0.90879999999999983</v>
+        <f t="shared" ref="O17" si="7">$E$16*$E$17*O16</f>
+        <v>0.8524799999999999</v>
       </c>
       <c r="P17">
-        <f t="shared" ref="P17" si="9">$E$16*$E$17*P16</f>
-        <v>0.54527999999999988</v>
+        <f t="shared" ref="P17" si="8">$E$16*$E$17*P16</f>
+        <v>0.51148799999999994</v>
       </c>
       <c r="Q17">
-        <f t="shared" ref="Q17" si="10">$E$16*$E$17*Q16</f>
-        <v>0.32716800000000024</v>
+        <f t="shared" ref="Q17" si="9">$E$16*$E$17*Q16</f>
+        <v>0.30689280000000024</v>
       </c>
       <c r="R17">
-        <f t="shared" ref="R17" si="11">$E$16*$E$17*R16</f>
-        <v>0.3271679999999999</v>
+        <f t="shared" ref="R17" si="10">$E$16*$E$17*R16</f>
+        <v>0.30689279999999991</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2760,48 +2772,48 @@
         <v>103</v>
       </c>
       <c r="H18" s="13">
-        <f>H17*E17</f>
-        <v>0.22719999999999999</v>
+        <f>PV($E$22,H15,,-H17)</f>
+        <v>0.53280000000000005</v>
       </c>
       <c r="I18" s="13">
-        <f>NPV($E$22,I17)+$H$18</f>
-        <v>1.0609614678899082</v>
+        <f t="shared" ref="I18:M18" si="11">PV($E$22,I15,,-I17)</f>
+        <v>0.79671028037383174</v>
       </c>
       <c r="J18" s="13">
-        <f>NPV($E$22,$I$17:J17)+$H$18</f>
-        <v>1.5199127346182981</v>
+        <f t="shared" si="11"/>
+        <v>0.44675342824700853</v>
       </c>
       <c r="K18" s="13">
-        <f>NPV($E$22,$I$17:K17)+$H$18</f>
-        <v>1.7725464594229163</v>
+        <f t="shared" si="11"/>
+        <v>0.25051594107308883</v>
       </c>
       <c r="L18" s="13">
-        <f>NPV($E$22,$I$17:L17)+$H$18</f>
-        <v>2.0043205188766944</v>
+        <f t="shared" si="11"/>
+        <v>0.23412704773185877</v>
       </c>
       <c r="M18" s="13">
-        <f>NPV($E$22,$I$17:M17)+$H$18</f>
-        <v>2.1106388947729231</v>
+        <f t="shared" si="11"/>
+        <v>0.10940516249152295</v>
       </c>
       <c r="N18" s="13">
         <f>NPV($E$22,$I$17:N17)/(1+$E$22)+M18</f>
-        <v>4.1492799373787186</v>
+        <v>2.1585070286286712</v>
       </c>
       <c r="O18" s="13">
         <f>NPV($E$22,$I$17:O17)/(1+$E$22)+N18</f>
-        <v>6.6440170549511262</v>
+        <v>4.7037600162254236</v>
       </c>
       <c r="P18" s="13">
         <f>NPV($E$22,$I$17:P17)/(1+$E$22)+O18</f>
-        <v>9.3898162321381822</v>
+        <v>7.5272285859490564</v>
       </c>
       <c r="Q18" s="13">
         <f>NPV($E$22,$I$17:Q17)/(1+$E$22)+P18</f>
-        <v>12.273814708195687</v>
+        <v>10.506705893313931</v>
       </c>
       <c r="R18" s="13">
         <f>NPV($E$22,$I$17:R17)/(1+$E$22)+Q18</f>
-        <v>15.284601531840758</v>
+        <v>13.631985759222022</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2818,9 +2830,40 @@
       </c>
       <c r="E19" s="15">
         <f>E16/E15</f>
-        <v>1.42</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>7.4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H19" s="13">
+        <f t="shared" ref="H19:L19" si="12">SUM(C18:H18)</f>
+        <v>0.53280000000000005</v>
+      </c>
+      <c r="I19" s="13">
+        <f t="shared" si="12"/>
+        <v>1.3295102803738317</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" si="12"/>
+        <v>1.7762637086208402</v>
+      </c>
+      <c r="K19" s="13">
+        <f t="shared" si="12"/>
+        <v>2.0267796496939292</v>
+      </c>
+      <c r="L19" s="13">
+        <f t="shared" si="12"/>
+        <v>2.2609066974257881</v>
+      </c>
+      <c r="M19" s="13">
+        <f>SUM(H18:M18)</f>
+        <v>2.3703118599173112</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -2834,56 +2877,11 @@
       <c r="D20" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="20">
         <f>E19*E17</f>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f>($E$16/$E$15)*($E$17)</f>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="J20">
-        <f t="shared" ref="J20:R20" si="12">($E$16/$E$15)*($E$17)</f>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="12"/>
-        <v>0.56799999999999995</v>
-      </c>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -2892,52 +2890,51 @@
       <c r="D21" s="22"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="H21" s="15">
-        <f>PV($E$22,H15,-H20)</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="15">
-        <f t="shared" ref="I21:M21" si="13">PV($E$22,I15,-I20)</f>
-        <v>0.52110091743119313</v>
-      </c>
-      <c r="J21" s="15">
+      <c r="G21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>($E$16/$E$15)*($E$17)</f>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21:R21" si="13">($E$16/$E$15)*($E$17)</f>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="13"/>
-        <v>0.99917515360659936</v>
-      </c>
-      <c r="K21" s="15">
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="13"/>
-        <v>1.4377753702812839</v>
-      </c>
-      <c r="L21" s="15">
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="M21">
         <f t="shared" si="13"/>
-        <v>1.8401608901663158</v>
-      </c>
-      <c r="M21" s="20">
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="13"/>
-        <v>2.2093219175837766</v>
-      </c>
-      <c r="N21" s="20">
-        <f t="shared" ref="N21" si="14">PV($E$22,N15,-N20)</f>
-        <v>2.548001759251171</v>
-      </c>
-      <c r="O21" s="20">
-        <f t="shared" ref="O21" si="15">PV($E$22,O15,-O20)</f>
-        <v>2.8587172103221752</v>
-      </c>
-      <c r="P21" s="20">
-        <f t="shared" ref="P21" si="16">PV($E$22,P15,-P20)</f>
-        <v>3.1437772571763074</v>
-      </c>
-      <c r="Q21" s="20">
-        <f t="shared" ref="Q21:R21" si="17">PV($E$22,Q15,-Q20)</f>
-        <v>3.4053002359415672</v>
-      </c>
-      <c r="R21" s="20">
-        <f t="shared" si="17"/>
-        <v>3.6452295742583192</v>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="13"/>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="13"/>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="13"/>
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="13"/>
+        <v>2.6640000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -2951,16 +2948,57 @@
       <c r="D22" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="52">
-        <v>0.09</v>
+      <c r="E22" s="51">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
+      <c r="G22" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="15">
+        <f>PV($E$22,H15,-H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="15">
+        <f>PV($E$22,I15,-I21)</f>
+        <v>2.4897196261682262</v>
+      </c>
+      <c r="J22" s="15">
+        <f>PV($E$22,J15,-J21)</f>
+        <v>4.8165603982880603</v>
+      </c>
+      <c r="K22" s="15">
+        <f>PV($E$22,K15,-K21)</f>
+        <v>6.9911779423252911</v>
+      </c>
+      <c r="L22" s="15">
+        <f>PV($E$22,L15,-L21)</f>
+        <v>9.0235307872198955</v>
+      </c>
+      <c r="M22" s="20">
+        <f>PV($E$22,M15,-M21)</f>
+        <v>10.922925969364393</v>
+      </c>
+      <c r="N22" s="20">
+        <f>PV($E$22,N15,-N21)</f>
+        <v>12.698061653611578</v>
+      </c>
+      <c r="O22" s="20">
+        <f>PV($E$22,O15,-O21)</f>
+        <v>14.35706696599213</v>
+      </c>
+      <c r="P22" s="20">
+        <f>PV($E$22,P15,-P21)</f>
+        <v>15.907539220553392</v>
+      </c>
+      <c r="Q22" s="20">
+        <f>PV($E$22,Q15,-Q21)</f>
+        <v>17.356578710797567</v>
+      </c>
+      <c r="R22" s="20">
+        <f>PV($E$22,R15,-R21)</f>
+        <v>18.710821225044455</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2978,7 +3016,6 @@
       <c r="J23" s="15"/>
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3102,6 +3139,13 @@
         <f>B28+B29</f>
         <v>-167599.59999999986</v>
       </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -3136,22 +3180,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.28515625" customWidth="1"/>
+    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3168,12 +3213,12 @@
       <c r="H1" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
       <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3526,7 +3571,7 @@
         <v>122</v>
       </c>
       <c r="B12" s="15">
-        <v>50000</v>
+        <v>54000</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3547,44 +3592,44 @@
         <v>0</v>
       </c>
       <c r="C13" s="9">
-        <f>-$B$12*(1-$B$32)</f>
-        <v>-30000</v>
+        <f>-$B$12*(1-$B$34)</f>
+        <v>-32400</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" ref="D13:L13" si="3">-$B$12*(1-$B$32)</f>
-        <v>-30000</v>
+        <f t="shared" ref="D13:L13" si="3">-$B$12*(1-$B$34)</f>
+        <v>-32400</v>
       </c>
       <c r="E13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="G13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="J13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="K13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
       <c r="L13" s="9">
         <f t="shared" si="3"/>
-        <v>-30000</v>
+        <v>-32400</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3593,44 +3638,44 @@
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9">
-        <f>NPV($B$33,C13)+$B$13</f>
-        <v>-28037.383177570093</v>
+        <f>NPV($B$35,C13)+$B$13</f>
+        <v>-29999.999999999996</v>
       </c>
       <c r="D14" s="9">
-        <f>NPV($B$33,$C$13:D13)+$B$13</f>
-        <v>-54240.545025766442</v>
+        <f>NPV($B$35,$C$13:D13)+$B$13</f>
+        <v>-57777.777777777774</v>
       </c>
       <c r="E14" s="9">
-        <f>NPV($B$33,$C$13:E13)+$B$13</f>
-        <v>-78729.481332492011</v>
+        <f>NPV($B$35,$C$13:E13)+$B$13</f>
+        <v>-83497.942386831273</v>
       </c>
       <c r="F14" s="9">
-        <f>NPV($B$33,$C$13:F13)+$B$13</f>
-        <v>-101616.33769391775</v>
+        <f>NPV($B$35,$C$13:F13)+$B$13</f>
+        <v>-107312.90961743635</v>
       </c>
       <c r="G14" s="9">
-        <f>NPV($B$33,$C$13:G13)+$B$13</f>
-        <v>-123005.92307842782</v>
+        <f>NPV($B$35,$C$13:G13)+$B$13</f>
+        <v>-129363.80520132995</v>
       </c>
       <c r="H14" s="9">
-        <f>NPV($B$33,$C$13:H13)+$B$13</f>
-        <v>-142996.18979292319</v>
+        <f>NPV($B$35,$C$13:H13)+$B$13</f>
+        <v>-149781.30111234254</v>
       </c>
       <c r="I14" s="9">
-        <f>NPV($B$33,$C$13:I13)+$B$13</f>
-        <v>-161678.68204946091</v>
+        <f>NPV($B$35,$C$13:I13)+$B$13</f>
+        <v>-168686.38991883566</v>
       </c>
       <c r="J14" s="9">
-        <f>NPV($B$33,$C$13:J13)+$B$13</f>
-        <v>-179138.95518641206</v>
+        <f>NPV($B$35,$C$13:J13)+$B$13</f>
+        <v>-186191.10177669968</v>
       </c>
       <c r="K14" s="9">
-        <f>NPV($B$33,$C$13:K13)+$B$13</f>
-        <v>-195456.96746393648</v>
+        <f>NPV($B$35,$C$13:K13)+$B$13</f>
+        <v>-202399.16831175896</v>
       </c>
       <c r="L14" s="9">
-        <f>NPV($B$33,$C$13:L13)+$B$13</f>
-        <v>-210707.44622797801</v>
+        <f>NPV($B$35,$C$13:L13)+$B$13</f>
+        <v>-217406.63732570273</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3649,7 +3694,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16" s="2">
         <v>7</v>
@@ -3665,13 +3710,13 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>126</v>
       </c>
       <c r="B17" s="15">
         <f>B18/B16</f>
-        <v>22142.857142857141</v>
+        <v>23571.428571428572</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -3684,132 +3729,132 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B18" s="15">
-        <v>155000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>165000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B19" s="15">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B20" s="15">
         <f>-B18</f>
-        <v>-155000</v>
+        <v>-165000</v>
       </c>
       <c r="C20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" ref="C20:I20" si="4">-$B$19*(1-$B$34)+($B$17*$B$34)</f>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="D20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" si="4"/>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="E20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" si="4"/>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="F20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" si="4"/>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="G20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" si="4"/>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="H20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" si="4"/>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="I20" s="15">
-        <f>-$B$19*(1-$B$32)+($B$17*$B$32)</f>
-        <v>-4942.8571428571431</v>
+        <f t="shared" si="4"/>
+        <v>-3171.4285714285706</v>
       </c>
       <c r="J20" s="15">
-        <f>-$B$19*(1-$B$32)</f>
-        <v>-13800</v>
+        <f>-$B$19*(1-$B$34)</f>
+        <v>-12600</v>
       </c>
       <c r="K20" s="15">
-        <f t="shared" ref="K20:L20" si="4">-$B$19*(1-$B$32)</f>
-        <v>-13800</v>
+        <f t="shared" ref="K20:L20" si="5">-$B$19*(1-$B$34)</f>
+        <v>-12600</v>
       </c>
       <c r="L20" s="15">
-        <f t="shared" si="4"/>
-        <v>-13800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-12600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15">
-        <f>NPV($B$33,C20) +$B$20</f>
-        <v>-159619.49265687584</v>
+        <f>NPV($B$35,C20) +$B$20</f>
+        <v>-167936.50793650793</v>
       </c>
       <c r="D21" s="15">
-        <f>NPV($B$33,$C$20:D20) +$B$20</f>
-        <v>-163936.77551376913</v>
+        <f>NPV($B$35,$C$20:D20) +$B$20</f>
+        <v>-170655.49676660789</v>
       </c>
       <c r="E21" s="15">
-        <f>NPV($B$33,$C$20:E20) +$B$20</f>
-        <v>-167971.61930525821</v>
+        <f>NPV($B$35,$C$20:E20) +$B$20</f>
+        <v>-173173.07901670042</v>
       </c>
       <c r="F21" s="15">
-        <f>NPV($B$33,$C$20:F20) +$B$20</f>
-        <v>-171742.50135337882</v>
+        <f>NPV($B$35,$C$20:F20) +$B$20</f>
+        <v>-175504.17369271201</v>
       </c>
       <c r="G21" s="15">
-        <f>NPV($B$33,$C$20:G20) +$B$20</f>
-        <v>-175266.69018339811</v>
+        <f>NPV($B$35,$C$20:G20) +$B$20</f>
+        <v>-177662.59468901905</v>
       </c>
       <c r="H21" s="15">
-        <f>NPV($B$33,$C$20:H20) +$B$20</f>
-        <v>-178560.32460397686</v>
+        <f>NPV($B$35,$C$20:H20) +$B$20</f>
+        <v>-179661.13264856263</v>
       </c>
       <c r="I21" s="15">
-        <f>NPV($B$33,$C$20:I20) +$B$20</f>
-        <v>-181638.48761386354</v>
+        <f>NPV($B$35,$C$20:I20) +$B$20</f>
+        <v>-181511.6307592511</v>
       </c>
       <c r="J21" s="15">
-        <f>NPV($B$33,$C$20:J20) +$B$20</f>
-        <v>-189670.21325686108</v>
+        <f>NPV($B$35,$C$20:J20) +$B$20</f>
+        <v>-188319.01870397601</v>
       </c>
       <c r="K21" s="15">
-        <f>NPV($B$33,$C$20:K20) +$B$20</f>
-        <v>-197176.49890452233</v>
+        <f>NPV($B$35,$C$20:K20) +$B$20</f>
+        <v>-194622.15568983238</v>
       </c>
       <c r="L21" s="15">
-        <f>NPV($B$33,$C$20:L20) +$B$20</f>
-        <v>-204191.71913598143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <f>NPV($B$35,$C$20:L20) +$B$20</f>
+        <v>-200458.39363969941</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B23" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>126</v>
       </c>
       <c r="B24" s="15">
         <f>B25/B23</f>
-        <v>35714.285714285717</v>
+        <v>36428.571428571428</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3822,171 +3867,189 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B25" s="15">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>255000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B26" s="15">
-        <v>39000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B27" s="15">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="15">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B30" s="15">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="15">
-        <f>-B25-(B26*B32)</f>
-        <v>-265600</v>
-      </c>
-      <c r="C29" s="15">
-        <f>(-$B$28)*(1-$B$32)+$B$24*$B$32+$B$27*$B$32</f>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="D29" s="15">
-        <f t="shared" ref="D29:L29" si="5">(-$B$28)*(1-$B$32)+$B$24*$B$32+$B$27*$B$32</f>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="E29" s="15">
-        <f t="shared" si="5"/>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="F29" s="15">
-        <f t="shared" si="5"/>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="G29" s="15">
-        <f t="shared" si="5"/>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="H29" s="15">
-        <f t="shared" si="5"/>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="I29" s="15">
-        <f t="shared" si="5"/>
-        <v>10885.714285714288</v>
-      </c>
-      <c r="J29" s="15">
-        <f>(-$B$28)*(1-$B$32)+$B$27*$B$32</f>
-        <v>-3400</v>
-      </c>
-      <c r="K29" s="15">
-        <f t="shared" ref="K29:L29" si="6">(-$B$28)*(1-$B$32)+$B$27*$B$32</f>
-        <v>-3400</v>
-      </c>
-      <c r="L29" s="15">
+      <c r="B31" s="15">
+        <f>-B25-B27-(B26*(1-B34))</f>
+        <v>-276600</v>
+      </c>
+      <c r="C31" s="15">
+        <f>($B$28-$B$30)*(1-$B$34)+($B$24*$B$34)</f>
+        <v>10971.428571428572</v>
+      </c>
+      <c r="D31" s="15">
+        <f t="shared" ref="D31:L31" si="6">($B$28-$B$30)*(1-$B$34)+($B$24*$B$34)</f>
+        <v>10971.428571428572</v>
+      </c>
+      <c r="E31" s="15">
         <f t="shared" si="6"/>
-        <v>-3400</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+        <v>10971.428571428572</v>
+      </c>
+      <c r="F31" s="15">
+        <f t="shared" si="6"/>
+        <v>10971.428571428572</v>
+      </c>
+      <c r="G31" s="15">
+        <f>($B$28-$B$30)*(1-$B$34)+($B$24*$B$34)</f>
+        <v>10971.428571428572</v>
+      </c>
+      <c r="H31" s="15">
+        <f t="shared" si="6"/>
+        <v>10971.428571428572</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" si="6"/>
+        <v>10971.428571428572</v>
+      </c>
+      <c r="J31" s="15">
+        <f>($B$28-$B$30)*(1-$B$34)</f>
+        <v>-3600</v>
+      </c>
+      <c r="K31" s="15">
+        <f t="shared" ref="K31:L31" si="7">($B$28-$B$30)*(1-$B$34)</f>
+        <v>-3600</v>
+      </c>
+      <c r="L31" s="15">
+        <f t="shared" si="7"/>
+        <v>-3600</v>
+      </c>
+      <c r="M31" s="15"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15">
-        <f>NPV($B$33,C29) +$B$29</f>
-        <v>-255426.435246996</v>
-      </c>
-      <c r="D30" s="15">
-        <f>NPV($B$33,$C$29:D29) +$B$29</f>
-        <v>-245918.43080493616</v>
-      </c>
-      <c r="E30" s="15">
-        <f>NPV($B$33,$C$29:E29) +$B$29</f>
-        <v>-237032.44534506719</v>
-      </c>
-      <c r="F30" s="15">
-        <f>NPV($B$33,$C$29:F29) +$B$29</f>
-        <v>-228727.78603677842</v>
-      </c>
-      <c r="G30" s="15">
-        <f>NPV($B$33,$C$29:G29) +$B$29</f>
-        <v>-220966.42219725618</v>
-      </c>
-      <c r="H30" s="15">
-        <f>NPV($B$33,$C$29:H29) +$B$29</f>
-        <v>-213712.81113228214</v>
-      </c>
-      <c r="I30" s="15">
-        <f>NPV($B$33,$C$29:I29) +$B$29</f>
-        <v>-206933.73537062417</v>
-      </c>
-      <c r="J30" s="15">
-        <f>NPV($B$33,$C$29:J29) +$B$29</f>
-        <v>-208912.56632614529</v>
-      </c>
-      <c r="K30" s="15">
-        <f>NPV($B$33,$C$29:K29) +$B$29</f>
-        <v>-210761.9410509314</v>
-      </c>
-      <c r="L30" s="15">
-        <f>NPV($B$33,$C$29:L29) +$B$29</f>
-        <v>-212490.32864418943</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15">
+        <f>NPV($B$35,C31) +$B$31</f>
+        <v>-266441.26984126982</v>
+      </c>
+      <c r="D32" s="15">
+        <f>NPV($B$35,$C$31:D31) +$B$31</f>
+        <v>-257035.038212816</v>
+      </c>
+      <c r="E32" s="15">
+        <f>NPV($B$35,$C$31:E31) +$B$31</f>
+        <v>-248325.56448276615</v>
+      </c>
+      <c r="F32" s="15">
+        <f>NPV($B$35,$C$31:F31) +$B$31</f>
+        <v>-240261.23695494217</v>
+      </c>
+      <c r="G32" s="15">
+        <f>NPV($B$35,$C$31:G31) +$B$31</f>
+        <v>-232794.26702177187</v>
+      </c>
+      <c r="H32" s="15">
+        <f>NPV($B$35,$C$31:H31) +$B$31</f>
+        <v>-225880.40597254009</v>
+      </c>
+      <c r="I32" s="15">
+        <f>NPV($B$35,$C$31:I31) +$B$31</f>
+        <v>-219478.68277880695</v>
+      </c>
+      <c r="J32" s="15">
+        <f>NPV($B$35,$C$31:J31) +$B$31</f>
+        <v>-221423.65076301407</v>
+      </c>
+      <c r="K32" s="15">
+        <f>NPV($B$35,$C$31:K31) +$B$31</f>
+        <v>-223224.54704468732</v>
+      </c>
+      <c r="L32" s="15">
+        <f>NPV($B$35,$C$31:L31) +$B$31</f>
+        <v>-224892.04360179219</v>
+      </c>
+      <c r="M32" s="15"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="52">
+      <c r="B34" s="51">
         <v>0.4</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B33" s="52">
-        <v>7.0000000000000007E-2</v>
+      <c r="B35" s="51">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>
@@ -4017,41 +4080,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="55">
-        <v>0</v>
-      </c>
-      <c r="C1" s="55">
+      <c r="B1" s="54">
+        <v>0</v>
+      </c>
+      <c r="C1" s="54">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="58"/>
+      <c r="B2" s="57"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="57"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="57">
         <v>33.200000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="58">
+      <c r="B5" s="57">
         <v>91.2</v>
       </c>
       <c r="C5" s="9">
@@ -4060,18 +4123,18 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B6" s="57">
         <v>168.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
+      <c r="A7" s="53"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="3">
@@ -4079,7 +4142,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="53" t="s">
         <v>109</v>
       </c>
       <c r="B9" s="3">
@@ -4087,26 +4150,26 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="57">
+      <c r="B10" s="56">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="57">
+      <c r="B11" s="56">
         <v>5.4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
+      <c r="A12" s="53"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="52" t="s">
         <v>117</v>
       </c>
       <c r="B13" s="9"/>
@@ -4116,7 +4179,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="53" t="s">
         <v>115</v>
       </c>
       <c r="B14" s="9"/>
@@ -4126,7 +4189,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="52" t="s">
         <v>116</v>
       </c>
       <c r="C15" s="9">

</xml_diff>